<commit_message>
Add first result plots
</commit_message>
<xml_diff>
--- a/Data/subject_list.xlsx
+++ b/Data/subject_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\pc\Dokumenter\PhD\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{765C91CF-098E-4056-BD7B-88CFED2D4994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F88F5FFC-8B1B-4486-82E7-A3B7DD494E5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23016" yWindow="5016" windowWidth="23016" windowHeight="12336" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="by student count" sheetId="1" r:id="rId1"/>
@@ -5561,8 +5561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86535E3C-402E-45BA-B91F-5268FA910A2C}">
   <dimension ref="A1:F201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="E103" sqref="E103"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E100" sqref="E100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>